<commit_message>
trying to incorporate non road sales shares
</commit_message>
<xml_diff>
--- a/input_data/fuel_mixing_assumptions.xlsx
+++ b/input_data/fuel_mixing_assumptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APERC\transport_model_9th_edition\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB79C6F5-0341-4868-9F17-E613B226A10E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E530130-1934-41E5-BC97-34239ACF7034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1755" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="927" activeTab="1" xr2:uid="{BD5D0853-27AB-4388-BA7A-28E1329E6022}"/>
   </bookViews>
@@ -1340,14 +1340,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H416"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H64" sqref="H64"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="41.1796875" customWidth="1"/>
-    <col min="3" max="3" width="25.08984375" customWidth="1"/>
+    <col min="3" max="3" width="25.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -1857,10 +1857,10 @@
         <v>44</v>
       </c>
       <c r="D25">
-        <v>2100</v>
+        <v>2070</v>
       </c>
       <c r="E25">
-        <v>0.34</v>
+        <v>0.15</v>
       </c>
       <c r="F25">
         <v>0.34</v>
@@ -2017,10 +2017,10 @@
         <v>44</v>
       </c>
       <c r="D33">
-        <v>2100</v>
+        <v>2070</v>
       </c>
       <c r="E33">
-        <v>0.34</v>
+        <v>0.15</v>
       </c>
       <c r="F33">
         <v>0.34</v>
@@ -2177,10 +2177,10 @@
         <v>44</v>
       </c>
       <c r="D41">
-        <v>2100</v>
+        <v>2070</v>
       </c>
       <c r="E41">
-        <v>0.34</v>
+        <v>0.15</v>
       </c>
       <c r="F41">
         <v>0.34</v>

</xml_diff>

<commit_message>
fixed non energy use sales being halved
</commit_message>
<xml_diff>
--- a/input_data/fuel_mixing_assumptions.xlsx
+++ b/input_data/fuel_mixing_assumptions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APERC\transport_model_9th_edition\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC67FD9-40B0-4449-9A4F-5D19D1227056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7F3020-823F-4D09-9B57-304845B14A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26805" yWindow="-15915" windowWidth="56460" windowHeight="14865" tabRatio="927" activeTab="1" xr2:uid="{BD5D0853-27AB-4388-BA7A-28E1329E6022}"/>
+    <workbookView xWindow="1755" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="927" activeTab="1" xr2:uid="{BD5D0853-27AB-4388-BA7A-28E1329E6022}"/>
   </bookViews>
   <sheets>
     <sheet name="regions" sheetId="1" r:id="rId1"/>
@@ -1340,8 +1340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J412"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C122" sqref="C122"/>
+    <sheetView tabSelected="1" topLeftCell="A193" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C219" sqref="C219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5095,10 +5095,10 @@
         <v>2021</v>
       </c>
       <c r="E186">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="F186">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="187" spans="1:10" x14ac:dyDescent="0.35">
@@ -5158,7 +5158,7 @@
         <v>0.05</v>
       </c>
       <c r="F189">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="190" spans="1:10" x14ac:dyDescent="0.35">
@@ -5178,7 +5178,7 @@
         <v>0.05</v>
       </c>
       <c r="F190">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="191" spans="1:10" x14ac:dyDescent="0.35">
@@ -5195,10 +5195,10 @@
         <v>2021</v>
       </c>
       <c r="E191">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="F191">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="192" spans="1:10" x14ac:dyDescent="0.35">
@@ -5258,7 +5258,7 @@
         <v>0.05</v>
       </c>
       <c r="F194">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.35">
@@ -5278,7 +5278,7 @@
         <v>0.05</v>
       </c>
       <c r="F195">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.35">
@@ -5295,10 +5295,10 @@
         <v>2021</v>
       </c>
       <c r="E196">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="F196">
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.35">
@@ -5358,7 +5358,7 @@
         <v>0.05</v>
       </c>
       <c r="F199">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.35">
@@ -5375,10 +5375,10 @@
         <v>2100</v>
       </c>
       <c r="E200">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="F200">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.35">
@@ -5458,7 +5458,7 @@
         <v>0.05</v>
       </c>
       <c r="F204">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.35">
@@ -5475,10 +5475,10 @@
         <v>2100</v>
       </c>
       <c r="E205">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="F205">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.35">
@@ -5558,7 +5558,7 @@
         <v>0.05</v>
       </c>
       <c r="F209">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.35">
@@ -5575,10 +5575,10 @@
         <v>2100</v>
       </c>
       <c r="E210">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="F210">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.35">
@@ -5598,7 +5598,7 @@
         <v>0</v>
       </c>
       <c r="F211">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.35">
@@ -5618,7 +5618,7 @@
         <v>0.01</v>
       </c>
       <c r="F212">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.35">
@@ -5638,7 +5638,7 @@
         <v>0.05</v>
       </c>
       <c r="F213">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.35">
@@ -5655,10 +5655,10 @@
         <v>2040</v>
       </c>
       <c r="E214">
+        <v>0.05</v>
+      </c>
+      <c r="F214">
         <v>0.1</v>
-      </c>
-      <c r="F214">
-        <v>0.02</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.35">
@@ -5675,10 +5675,10 @@
         <v>2100</v>
       </c>
       <c r="E215">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="F215">
-        <v>0.02</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.35">
@@ -5698,7 +5698,7 @@
         <v>0</v>
       </c>
       <c r="F216">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.35">
@@ -5718,7 +5718,7 @@
         <v>0.01</v>
       </c>
       <c r="F217">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.35">
@@ -5738,7 +5738,7 @@
         <v>0.05</v>
       </c>
       <c r="F218">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.35">
@@ -5755,10 +5755,10 @@
         <v>2040</v>
       </c>
       <c r="E219">
+        <v>0.05</v>
+      </c>
+      <c r="F219">
         <v>0.1</v>
-      </c>
-      <c r="F219">
-        <v>0.02</v>
       </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.35">
@@ -5775,10 +5775,10 @@
         <v>2100</v>
       </c>
       <c r="E220">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="F220">
-        <v>0.02</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.35">
@@ -5818,7 +5818,7 @@
         <v>0.01</v>
       </c>
       <c r="F222">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.35">
@@ -5838,7 +5838,7 @@
         <v>0.05</v>
       </c>
       <c r="F223">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.35">
@@ -5858,7 +5858,7 @@
         <v>0.1</v>
       </c>
       <c r="F224">
-        <v>0.02</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.35">
@@ -5878,7 +5878,7 @@
         <v>0.3</v>
       </c>
       <c r="F225">
-        <v>0.02</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.35">
@@ -5918,7 +5918,7 @@
         <v>0.01</v>
       </c>
       <c r="F227">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.35">
@@ -5938,7 +5938,7 @@
         <v>0.05</v>
       </c>
       <c r="F228">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.35">
@@ -5958,7 +5958,7 @@
         <v>0.1</v>
       </c>
       <c r="F229">
-        <v>0.02</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.35">
@@ -5978,7 +5978,7 @@
         <v>0.3</v>
       </c>
       <c r="F230">
-        <v>0.02</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.35">
@@ -6018,7 +6018,7 @@
         <v>0.01</v>
       </c>
       <c r="F232">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.35">
@@ -6038,7 +6038,7 @@
         <v>0.05</v>
       </c>
       <c r="F233">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.35">
@@ -6058,7 +6058,7 @@
         <v>0.1</v>
       </c>
       <c r="F234">
-        <v>0.02</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.35">
@@ -6078,7 +6078,7 @@
         <v>0.3</v>
       </c>
       <c r="F235">
-        <v>0.02</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.35">
@@ -6118,7 +6118,7 @@
         <v>0.01</v>
       </c>
       <c r="F237">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.35">
@@ -6138,7 +6138,7 @@
         <v>0.05</v>
       </c>
       <c r="F238">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.35">
@@ -6158,7 +6158,7 @@
         <v>0.1</v>
       </c>
       <c r="F239">
-        <v>0.02</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.35">
@@ -6178,7 +6178,7 @@
         <v>0.3</v>
       </c>
       <c r="F240">
-        <v>0.02</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
bunkers ready. needs work though
</commit_message>
<xml_diff>
--- a/input_data/fuel_mixing_assumptions.xlsx
+++ b/input_data/fuel_mixing_assumptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\APERC\transport_model_9th_edition\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D989FBA9-D8DE-4872-8A5A-33FF6F6A97AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21814D45-AE13-46BF-B4AE-1135A5550C82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" tabRatio="927" firstSheet="2" activeTab="2" xr2:uid="{BD5D0853-27AB-4388-BA7A-28E1329E6022}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <sheet name="demand_side_constant" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">international_supply_side!$A$1:$H$350</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">international_supply_side!$A$1:$H$347</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">supply_side!$A$1:$F$350</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1317" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1467" uniqueCount="84">
   <si>
     <t>Region</t>
   </si>
@@ -8720,10 +8720,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{199A55F7-775E-41E6-8F2F-58868FFF4869}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="D1:E1"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9014,10 +9014,790 @@
         <v>0.2</v>
       </c>
     </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" t="s">
+        <v>71</v>
+      </c>
+      <c r="F12">
+        <v>2040</v>
+      </c>
+      <c r="G12">
+        <v>0.1</v>
+      </c>
+      <c r="H12">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13">
+        <v>2040</v>
+      </c>
+      <c r="G13">
+        <v>0.1</v>
+      </c>
+      <c r="H13">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14">
+        <v>2040</v>
+      </c>
+      <c r="G14">
+        <v>0.1</v>
+      </c>
+      <c r="H14">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15">
+        <v>2040</v>
+      </c>
+      <c r="G15">
+        <v>0.1</v>
+      </c>
+      <c r="H15">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16">
+        <v>2040</v>
+      </c>
+      <c r="G16">
+        <v>0.1</v>
+      </c>
+      <c r="H16">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17">
+        <v>2040</v>
+      </c>
+      <c r="G17">
+        <v>0.1</v>
+      </c>
+      <c r="H17">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18">
+        <v>2040</v>
+      </c>
+      <c r="G18">
+        <v>0.1</v>
+      </c>
+      <c r="H18">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19">
+        <v>2040</v>
+      </c>
+      <c r="G19">
+        <v>0.1</v>
+      </c>
+      <c r="H19">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20">
+        <v>2040</v>
+      </c>
+      <c r="G20">
+        <v>0.1</v>
+      </c>
+      <c r="H20">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" t="s">
+        <v>83</v>
+      </c>
+      <c r="D21" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21">
+        <v>2040</v>
+      </c>
+      <c r="G21">
+        <v>0.1</v>
+      </c>
+      <c r="H21">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" t="s">
+        <v>73</v>
+      </c>
+      <c r="D22" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F22">
+        <v>2050</v>
+      </c>
+      <c r="G22">
+        <v>0.1</v>
+      </c>
+      <c r="H22">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" t="s">
+        <v>75</v>
+      </c>
+      <c r="D23" t="s">
+        <v>63</v>
+      </c>
+      <c r="E23" t="s">
+        <v>71</v>
+      </c>
+      <c r="F23">
+        <v>2050</v>
+      </c>
+      <c r="G23">
+        <v>0.1</v>
+      </c>
+      <c r="H23">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" t="s">
+        <v>42</v>
+      </c>
+      <c r="F24">
+        <v>2050</v>
+      </c>
+      <c r="G24">
+        <v>0.1</v>
+      </c>
+      <c r="H24">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" t="s">
+        <v>42</v>
+      </c>
+      <c r="F25">
+        <v>2050</v>
+      </c>
+      <c r="G25">
+        <v>0.1</v>
+      </c>
+      <c r="H25">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26" t="s">
+        <v>78</v>
+      </c>
+      <c r="D26" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F26">
+        <v>2050</v>
+      </c>
+      <c r="G26">
+        <v>0.1</v>
+      </c>
+      <c r="H26">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" t="s">
+        <v>79</v>
+      </c>
+      <c r="D27" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" t="s">
+        <v>43</v>
+      </c>
+      <c r="F27">
+        <v>2050</v>
+      </c>
+      <c r="G27">
+        <v>0.1</v>
+      </c>
+      <c r="H27">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" t="s">
+        <v>80</v>
+      </c>
+      <c r="D28" t="s">
+        <v>70</v>
+      </c>
+      <c r="E28" t="s">
+        <v>44</v>
+      </c>
+      <c r="F28">
+        <v>2050</v>
+      </c>
+      <c r="G28">
+        <v>0.1</v>
+      </c>
+      <c r="H28">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29" t="s">
+        <v>81</v>
+      </c>
+      <c r="D29" t="s">
+        <v>38</v>
+      </c>
+      <c r="E29" t="s">
+        <v>44</v>
+      </c>
+      <c r="F29">
+        <v>2050</v>
+      </c>
+      <c r="G29">
+        <v>0.1</v>
+      </c>
+      <c r="H29">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" t="s">
+        <v>82</v>
+      </c>
+      <c r="D30" t="s">
+        <v>39</v>
+      </c>
+      <c r="E30" t="s">
+        <v>44</v>
+      </c>
+      <c r="F30">
+        <v>2050</v>
+      </c>
+      <c r="G30">
+        <v>0.1</v>
+      </c>
+      <c r="H30">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" t="s">
+        <v>74</v>
+      </c>
+      <c r="C31" t="s">
+        <v>83</v>
+      </c>
+      <c r="D31" t="s">
+        <v>70</v>
+      </c>
+      <c r="E31" t="s">
+        <v>44</v>
+      </c>
+      <c r="F31">
+        <v>2050</v>
+      </c>
+      <c r="G31">
+        <v>0.1</v>
+      </c>
+      <c r="H31">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32" t="s">
+        <v>73</v>
+      </c>
+      <c r="D32" t="s">
+        <v>63</v>
+      </c>
+      <c r="E32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F32">
+        <v>2070</v>
+      </c>
+      <c r="G32">
+        <v>0.1</v>
+      </c>
+      <c r="H32">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33" t="s">
+        <v>74</v>
+      </c>
+      <c r="C33" t="s">
+        <v>75</v>
+      </c>
+      <c r="D33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E33" t="s">
+        <v>71</v>
+      </c>
+      <c r="F33">
+        <v>2070</v>
+      </c>
+      <c r="G33">
+        <v>0.1</v>
+      </c>
+      <c r="H33">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" t="s">
+        <v>76</v>
+      </c>
+      <c r="D34" t="s">
+        <v>37</v>
+      </c>
+      <c r="E34" t="s">
+        <v>42</v>
+      </c>
+      <c r="F34">
+        <v>2070</v>
+      </c>
+      <c r="G34">
+        <v>0.1</v>
+      </c>
+      <c r="H34">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>67</v>
+      </c>
+      <c r="B35" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" t="s">
+        <v>77</v>
+      </c>
+      <c r="D35" t="s">
+        <v>37</v>
+      </c>
+      <c r="E35" t="s">
+        <v>42</v>
+      </c>
+      <c r="F35">
+        <v>2070</v>
+      </c>
+      <c r="G35">
+        <v>0.1</v>
+      </c>
+      <c r="H35">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36" t="s">
+        <v>72</v>
+      </c>
+      <c r="C36" t="s">
+        <v>78</v>
+      </c>
+      <c r="D36" t="s">
+        <v>35</v>
+      </c>
+      <c r="E36" t="s">
+        <v>43</v>
+      </c>
+      <c r="F36">
+        <v>2070</v>
+      </c>
+      <c r="G36">
+        <v>0.1</v>
+      </c>
+      <c r="H36">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>67</v>
+      </c>
+      <c r="B37" t="s">
+        <v>74</v>
+      </c>
+      <c r="C37" t="s">
+        <v>79</v>
+      </c>
+      <c r="D37" t="s">
+        <v>35</v>
+      </c>
+      <c r="E37" t="s">
+        <v>43</v>
+      </c>
+      <c r="F37">
+        <v>2070</v>
+      </c>
+      <c r="G37">
+        <v>0.1</v>
+      </c>
+      <c r="H37">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>67</v>
+      </c>
+      <c r="B38" t="s">
+        <v>72</v>
+      </c>
+      <c r="C38" t="s">
+        <v>80</v>
+      </c>
+      <c r="D38" t="s">
+        <v>70</v>
+      </c>
+      <c r="E38" t="s">
+        <v>44</v>
+      </c>
+      <c r="F38">
+        <v>2070</v>
+      </c>
+      <c r="G38">
+        <v>0.1</v>
+      </c>
+      <c r="H38">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>67</v>
+      </c>
+      <c r="B39" t="s">
+        <v>74</v>
+      </c>
+      <c r="C39" t="s">
+        <v>81</v>
+      </c>
+      <c r="D39" t="s">
+        <v>38</v>
+      </c>
+      <c r="E39" t="s">
+        <v>44</v>
+      </c>
+      <c r="F39">
+        <v>2070</v>
+      </c>
+      <c r="G39">
+        <v>0.1</v>
+      </c>
+      <c r="H39">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>67</v>
+      </c>
+      <c r="B40" t="s">
+        <v>74</v>
+      </c>
+      <c r="C40" t="s">
+        <v>82</v>
+      </c>
+      <c r="D40" t="s">
+        <v>39</v>
+      </c>
+      <c r="E40" t="s">
+        <v>44</v>
+      </c>
+      <c r="F40">
+        <v>2070</v>
+      </c>
+      <c r="G40">
+        <v>0.1</v>
+      </c>
+      <c r="H40">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>67</v>
+      </c>
+      <c r="B41" t="s">
+        <v>74</v>
+      </c>
+      <c r="C41" t="s">
+        <v>83</v>
+      </c>
+      <c r="D41" t="s">
+        <v>70</v>
+      </c>
+      <c r="E41" t="s">
+        <v>44</v>
+      </c>
+      <c r="F41">
+        <v>2070</v>
+      </c>
+      <c r="G41">
+        <v>0.1</v>
+      </c>
+      <c r="H41">
+        <v>0.4</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:H350" xr:uid="{199A55F7-775E-41E6-8F2F-58868FFF4869}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H350">
-      <sortCondition ref="F1:F350"/>
+  <autoFilter ref="A1:H347" xr:uid="{199A55F7-775E-41E6-8F2F-58868FFF4869}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H347">
+      <sortCondition ref="F1:F347"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="D1:E1">

</xml_diff>